<commit_message>
Final Save Upload/Download 19-1-2023
</commit_message>
<xml_diff>
--- a/Extras/Book2.xlsx
+++ b/Extras/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeeld\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\MERN\Multer\Extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAED1E8-D9AA-415A-9D4B-0F95A9D304D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE44B2A5-B44D-427E-B2F0-9F6FC60724F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="708" yWindow="1152" windowWidth="7656" windowHeight="5304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
@@ -878,7 +878,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>